<commit_message>
MySQL automation package practic is added
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -502,9 +502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" activeCellId="1" sqref="D38 D38"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>

</xml_diff>